<commit_message>
small figure changes and doc with appendix tables
</commit_message>
<xml_diff>
--- a/doc/model results.xlsx
+++ b/doc/model results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Experiments/Move-along/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/movealong/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{98ABCBFD-7B43-43F9-A7A1-55688472F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A2A6D52-8CEB-4780-9647-465BFA71BCBB}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{98ABCBFD-7B43-43F9-A7A1-55688472F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A47955D8-A63F-4DE8-993F-C794CA8B90AF}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{B02C3BB0-3B4F-4AA3-A8CF-A5D428BFD4B8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{B02C3BB0-3B4F-4AA3-A8CF-A5D428BFD4B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Germ_rate" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="70">
   <si>
     <t>cumulative, viable - cumulative ~ incubator * time</t>
   </si>
@@ -234,15 +234,6 @@
     <t>autumn_germ, viable  -  autumn_germ  ~  incubator * community</t>
   </si>
   <si>
-    <t>t50lm ~ incubator*community</t>
-  </si>
-  <si>
-    <t>heat_sum ~ incubator*community</t>
-  </si>
-  <si>
-    <t>1..52</t>
-  </si>
-  <si>
     <t>&lt; 1e-04</t>
   </si>
   <si>
@@ -250,6 +241,18 @@
   </si>
   <si>
     <t>scale(t50) ~ incubator</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>population:species</t>
+  </si>
+  <si>
+    <t>scale (t50lm) ~ incubator*community</t>
+  </si>
+  <si>
+    <t>sacle(heat_sum) ~ incubator*community</t>
   </si>
 </sst>
 </file>
@@ -513,6 +516,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -814,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97AC48C0-7438-470B-8030-A36EBE1AD09C}">
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P32" activeCellId="1" sqref="P30:S30 P32:S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,7 +1205,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="C13">
         <v>1.79</v>
@@ -1224,10 +1231,10 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1.52</v>
       </c>
       <c r="D14" s="7">
         <v>0.67</v>
@@ -1587,7 +1594,7 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:E9"/>
+      <selection activeCell="C28" activeCellId="1" sqref="C26:E26 C28:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2149,7 +2156,7 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:H29"/>
+      <selection activeCell="C28" activeCellId="1" sqref="C26:E26 C28:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2355,7 +2362,7 @@
         <v>6958</v>
       </c>
       <c r="N6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O6" s="7" t="s">
         <v>44</v>
@@ -2733,8 +2740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C77618-B808-42C0-948C-81CC35016D49}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20:H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" activeCellId="1" sqref="C26:E26 C28:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3295,7 +3302,7 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:H29"/>
+      <selection activeCell="C28" activeCellId="1" sqref="C26:E26 C28:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3508,7 +3515,7 @@
         <v>9000</v>
       </c>
       <c r="N6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O6" s="7" t="s">
         <v>44</v>
@@ -3866,7 +3873,7 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:H30"/>
+      <selection activeCell="C28" activeCellId="1" sqref="C26:E26 C28:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4057,7 +4064,7 @@
         <v>8124</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>44</v>
@@ -4118,7 +4125,7 @@
         <v>0.69</v>
       </c>
       <c r="D9" s="7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E9" s="7">
         <v>0.97</v>
@@ -4435,8 +4442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9EDF82-FF20-46B4-B10B-18AF673773AE}">
   <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:H44"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C43" activeCellId="1" sqref="C41:E41 C43:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4623,7 +4630,7 @@
         <v>9000</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>44</v>
@@ -4806,7 +4813,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -5102,7 +5109,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B31" s="17" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -5155,22 +5162,19 @@
         <v>57</v>
       </c>
       <c r="C35">
-        <v>103.81</v>
+        <v>-0.30565999999999999</v>
       </c>
       <c r="D35">
-        <v>64.88</v>
+        <v>-0.70320000000000005</v>
       </c>
       <c r="E35">
-        <v>142.34</v>
+        <v>6.3420000000000004E-2</v>
       </c>
       <c r="F35">
-        <v>9507</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H35" s="13" t="s">
-        <v>44</v>
+        <v>9000</v>
+      </c>
+      <c r="G35">
+        <v>0.11688999999999999</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -5178,21 +5182,21 @@
         <v>17</v>
       </c>
       <c r="C36">
-        <v>37.24</v>
+        <v>0.33180999999999999</v>
       </c>
       <c r="D36">
-        <v>25.1</v>
+        <v>0.2248</v>
       </c>
       <c r="E36">
-        <v>49.45</v>
+        <v>0.44524000000000002</v>
       </c>
       <c r="F36">
-        <v>9000</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H36" s="13" t="s">
+        <v>8679</v>
+      </c>
+      <c r="G36" t="s">
+        <v>63</v>
+      </c>
+      <c r="H36" t="s">
         <v>44</v>
       </c>
     </row>
@@ -5201,22 +5205,22 @@
         <v>45</v>
       </c>
       <c r="C37">
-        <v>69.2</v>
+        <v>0.61665000000000003</v>
       </c>
       <c r="D37">
-        <v>31.35</v>
+        <v>0.25652999999999998</v>
       </c>
       <c r="E37">
-        <v>108.58</v>
+        <v>0.96257999999999999</v>
       </c>
       <c r="F37">
-        <v>9000</v>
-      </c>
-      <c r="G37" s="7">
-        <v>6.6699999999999995E-4</v>
-      </c>
-      <c r="H37" s="13" t="s">
-        <v>44</v>
+        <v>9229</v>
+      </c>
+      <c r="G37">
+        <v>1.1100000000000001E-3</v>
+      </c>
+      <c r="H37" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -5224,21 +5228,21 @@
         <v>46</v>
       </c>
       <c r="C38">
-        <v>41.35</v>
+        <v>0.37132999999999999</v>
       </c>
       <c r="D38">
-        <v>21.91</v>
+        <v>0.19386</v>
       </c>
       <c r="E38">
-        <v>60.94</v>
+        <v>0.55735999999999997</v>
       </c>
       <c r="F38">
-        <v>9000</v>
-      </c>
-      <c r="G38" s="7">
-        <v>2.22E-4</v>
-      </c>
-      <c r="H38" s="13" t="s">
+        <v>8578</v>
+      </c>
+      <c r="G38" t="s">
+        <v>63</v>
+      </c>
+      <c r="H38" t="s">
         <v>44</v>
       </c>
     </row>
@@ -5266,13 +5270,13 @@
         <v>24</v>
       </c>
       <c r="C41">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41">
-        <v>0.56000000000000005</v>
+        <v>0.61</v>
       </c>
       <c r="H41" s="4"/>
     </row>
@@ -5281,13 +5285,13 @@
         <v>25</v>
       </c>
       <c r="C42">
-        <v>1375.34</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>4014.71</v>
+        <v>0.4</v>
       </c>
       <c r="H42" s="4"/>
     </row>
@@ -5296,13 +5300,13 @@
         <v>26</v>
       </c>
       <c r="C43">
-        <v>932.34</v>
+        <v>0.09</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>3011.81</v>
+        <v>0.27</v>
       </c>
       <c r="H43" s="4"/>
     </row>
@@ -5311,13 +5315,13 @@
         <v>27</v>
       </c>
       <c r="C44" s="9">
-        <v>4770.26</v>
+        <v>0.38</v>
       </c>
       <c r="D44" s="9">
-        <v>2985.19</v>
+        <v>0.24</v>
       </c>
       <c r="E44" s="9">
-        <v>6821.15</v>
+        <v>0.54</v>
       </c>
       <c r="F44" s="15"/>
       <c r="G44" s="15"/>
@@ -5343,8 +5347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F0277B2-62A9-411E-8838-82E73478C0F2}">
   <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:H44"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C43" activeCellId="1" sqref="C41:E41 C43:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5711,7 +5715,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -6005,7 +6009,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -6049,19 +6053,19 @@
         <v>57</v>
       </c>
       <c r="C35">
-        <v>351.21699999999998</v>
+        <v>6.1771E-2</v>
       </c>
       <c r="D35">
-        <v>207.01400000000001</v>
+        <v>-0.39675100000000002</v>
       </c>
       <c r="E35">
-        <v>501.98399999999998</v>
+        <v>0.51835900000000001</v>
       </c>
       <c r="F35">
-        <v>8729</v>
+        <v>9000</v>
       </c>
       <c r="G35">
-        <v>2.22E-4</v>
+        <v>0.79730000000000001</v>
       </c>
       <c r="H35" t="s">
         <v>44</v>
@@ -6072,19 +6076,19 @@
         <v>17</v>
       </c>
       <c r="C36">
-        <v>-52.186</v>
+        <v>-0.14511599999999999</v>
       </c>
       <c r="D36">
-        <v>-102.008</v>
+        <v>-0.28266000000000002</v>
       </c>
       <c r="E36">
-        <v>-3.4119999999999999</v>
+        <v>-7.6340000000000002E-3</v>
       </c>
       <c r="F36">
         <v>9000</v>
       </c>
-      <c r="G36" s="7">
-        <v>4.1556000000000003E-2</v>
+      <c r="G36">
+        <v>4.2700000000000002E-2</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>47</v>
@@ -6095,19 +6099,19 @@
         <v>45</v>
       </c>
       <c r="C37">
-        <v>129.26900000000001</v>
+        <v>0.35073199999999999</v>
       </c>
       <c r="D37">
-        <v>-16.428999999999998</v>
+        <v>-6.3107999999999997E-2</v>
       </c>
       <c r="E37">
-        <v>279.44</v>
+        <v>0.79792099999999999</v>
       </c>
       <c r="F37">
-        <v>9000</v>
+        <v>8593</v>
       </c>
       <c r="G37">
-        <v>8.7110999999999994E-2</v>
+        <v>0.1133</v>
       </c>
       <c r="H37" t="s">
         <v>58</v>
@@ -6118,19 +6122,19 @@
         <v>46</v>
       </c>
       <c r="C38">
-        <v>87.37</v>
+        <v>0.25335999999999997</v>
       </c>
       <c r="D38">
-        <v>8.3179999999999996</v>
+        <v>2.4059000000000001E-2</v>
       </c>
       <c r="E38">
-        <v>168.262</v>
+        <v>0.46934300000000001</v>
       </c>
       <c r="F38">
-        <v>9000</v>
-      </c>
-      <c r="G38" s="7">
-        <v>3.4222000000000002E-2</v>
+        <v>9330</v>
+      </c>
+      <c r="G38">
+        <v>2.53E-2</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>47</v>
@@ -6155,13 +6159,13 @@
         <v>24</v>
       </c>
       <c r="C41">
-        <v>0.22</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41">
-        <v>0.52</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
@@ -6169,13 +6173,13 @@
         <v>25</v>
       </c>
       <c r="C42">
-        <v>18916.34</v>
+        <v>0.2</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>56639.45</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
@@ -6183,13 +6187,13 @@
         <v>26</v>
       </c>
       <c r="C43">
-        <v>13551.09</v>
+        <v>0.15</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>48706.77</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
@@ -6197,13 +6201,13 @@
         <v>27</v>
       </c>
       <c r="C44" s="7">
-        <v>75433.66</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D44" s="7">
-        <v>45660.19</v>
+        <v>0.34</v>
       </c>
       <c r="E44" s="7">
-        <v>110558.1</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
germiantion curves visualization sincronization data
</commit_message>
<xml_diff>
--- a/doc/model results.xlsx
+++ b/doc/model results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/movealong/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{98ABCBFD-7B43-43F9-A7A1-55688472F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A47955D8-A63F-4DE8-993F-C794CA8B90AF}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="13_ncr:1_{98ABCBFD-7B43-43F9-A7A1-55688472F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B805BB3-0143-40C6-BF70-546C1E68D9B8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{B02C3BB0-3B4F-4AA3-A8CF-A5D428BFD4B8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B02C3BB0-3B4F-4AA3-A8CF-A5D428BFD4B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Germ_rate" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="winter_germ" sheetId="5" r:id="rId6"/>
     <sheet name="t50" sheetId="6" r:id="rId7"/>
     <sheet name="heat_sum" sheetId="7" r:id="rId8"/>
+    <sheet name="sincronia" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="72">
   <si>
     <t>cumulative, viable - cumulative ~ incubator * time</t>
   </si>
@@ -253,6 +254,12 @@
   </si>
   <si>
     <t>sacle(heat_sum) ~ incubator*community</t>
+  </si>
+  <si>
+    <t>SYNCHRONY INDEX (GERMINAR PACKAGE)</t>
+  </si>
+  <si>
+    <t>phylogeny</t>
   </si>
 </sst>
 </file>
@@ -406,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -440,6 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,15 +476,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1504950</xdr:colOff>
+      <xdr:colOff>1352550</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>57151</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>23251</xdr:rowOff>
+      <xdr:rowOff>128026</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -505,7 +513,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2266950" y="2676524"/>
+          <a:off x="2114550" y="2781299"/>
           <a:ext cx="8867776" cy="4604777"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -821,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97AC48C0-7438-470B-8030-A36EBE1AD09C}">
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P32" activeCellId="1" sqref="P30:S30 P32:S33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,7 +1187,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="C12">
         <v>4.24</v>
@@ -1594,7 +1602,7 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" activeCellId="1" sqref="C26:E26 C28:E29"/>
+      <selection activeCell="K9" sqref="K9:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4442,8 +4450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9EDF82-FF20-46B4-B10B-18AF673773AE}">
   <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C43" activeCellId="1" sqref="C41:E41 C43:E44"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5347,7 +5355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F0277B2-62A9-411E-8838-82E73478C0F2}">
   <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C43" activeCellId="1" sqref="C41:E41 C43:E44"/>
     </sheetView>
   </sheetViews>
@@ -6224,4 +6232,559 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50ACBF76-44B5-4680-9A32-27A43CC564F5}">
+  <dimension ref="A1:R29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>-2.4479999999999998E-2</v>
+      </c>
+      <c r="D5">
+        <v>-0.61245000000000005</v>
+      </c>
+      <c r="E5">
+        <v>0.61119000000000001</v>
+      </c>
+      <c r="F5">
+        <v>9000</v>
+      </c>
+      <c r="G5">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5">
+        <v>0.20530000000000001</v>
+      </c>
+      <c r="K5">
+        <v>-0.24546999999999999</v>
+      </c>
+      <c r="L5">
+        <v>0.67357</v>
+      </c>
+      <c r="M5">
+        <v>9000</v>
+      </c>
+      <c r="N5">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>4.224E-2</v>
+      </c>
+      <c r="D6">
+        <v>-9.2410000000000006E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.19152</v>
+      </c>
+      <c r="F6">
+        <v>9427</v>
+      </c>
+      <c r="G6">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6">
+        <v>-2.5590000000000002E-2</v>
+      </c>
+      <c r="K6">
+        <v>-0.23857999999999999</v>
+      </c>
+      <c r="L6">
+        <v>0.17204</v>
+      </c>
+      <c r="M6">
+        <v>9000</v>
+      </c>
+      <c r="N6">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="O6" s="23"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>0.41</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.69</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9">
+        <v>0.24</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>0.42</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1.01</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10">
+        <v>0.26</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>0.18</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.09</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0.33</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="23">
+        <v>0.13</v>
+      </c>
+      <c r="K12" s="23">
+        <v>0</v>
+      </c>
+      <c r="L12" s="23">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20">
+        <v>0.19208</v>
+      </c>
+      <c r="D20">
+        <v>-0.18894</v>
+      </c>
+      <c r="E20">
+        <v>0.64039999999999997</v>
+      </c>
+      <c r="F20">
+        <v>9000</v>
+      </c>
+      <c r="G20">
+        <v>0.33400000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>4.87E-2</v>
+      </c>
+      <c r="D21">
+        <v>-0.10038999999999999</v>
+      </c>
+      <c r="E21">
+        <v>0.19105</v>
+      </c>
+      <c r="F21">
+        <v>9000</v>
+      </c>
+      <c r="G21">
+        <v>0.50780000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22">
+        <v>-0.33106999999999998</v>
+      </c>
+      <c r="D22">
+        <v>-0.66047</v>
+      </c>
+      <c r="E22">
+        <v>3.7190000000000001E-2</v>
+      </c>
+      <c r="F22">
+        <v>9000</v>
+      </c>
+      <c r="G22">
+        <v>6.7599999999999993E-2</v>
+      </c>
+      <c r="R22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23">
+        <v>-6.8339999999999998E-2</v>
+      </c>
+      <c r="D23">
+        <v>-0.29370000000000002</v>
+      </c>
+      <c r="E23">
+        <v>0.16388</v>
+      </c>
+      <c r="F23">
+        <v>9000</v>
+      </c>
+      <c r="G23">
+        <v>0.55069999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <v>0.21</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0.48</v>
+      </c>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>0.16</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0.45</v>
+      </c>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>0.2</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0.42</v>
+      </c>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="9">
+        <v>0.18</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="E29" s="9">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="I3:O3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
figures changes and Cerastium ramosissimum updated
</commit_message>
<xml_diff>
--- a/doc/model results.xlsx
+++ b/doc/model results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/movealong/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="13_ncr:1_{98ABCBFD-7B43-43F9-A7A1-55688472F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B805BB3-0143-40C6-BF70-546C1E68D9B8}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="13_ncr:1_{98ABCBFD-7B43-43F9-A7A1-55688472F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF5C68C6-C74B-4450-ADC1-C25A7EAF74C9}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B02C3BB0-3B4F-4AA3-A8CF-A5D428BFD4B8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{B02C3BB0-3B4F-4AA3-A8CF-A5D428BFD4B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Germ_rate" sheetId="1" r:id="rId1"/>
@@ -413,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -447,7 +447,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -829,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97AC48C0-7438-470B-8030-A36EBE1AD09C}">
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1602,7 +1601,7 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9:L9"/>
+      <selection activeCell="J10" activeCellId="1" sqref="C10:E10 J10:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2164,7 +2163,7 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" activeCellId="1" sqref="C26:E26 C28:E29"/>
+      <selection activeCell="J10" activeCellId="1" sqref="C10:E10 J10:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2749,7 +2748,7 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" activeCellId="1" sqref="C26:E26 C28:E29"/>
+      <selection activeCell="J10" activeCellId="1" sqref="C10:E10 J10:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3310,7 +3309,7 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" activeCellId="1" sqref="C26:E26 C28:E29"/>
+      <selection activeCell="J10" activeCellId="1" sqref="C10:E10 J10:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3881,7 +3880,7 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" activeCellId="1" sqref="C26:E26 C28:E29"/>
+      <selection activeCell="J10" activeCellId="1" sqref="C10:E10 J10:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4451,7 +4450,7 @@
   <dimension ref="A1:R44"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:O44"/>
+      <selection activeCell="G36" sqref="G36:H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5201,10 +5200,10 @@
       <c r="F36">
         <v>8679</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="7" t="s">
         <v>44</v>
       </c>
     </row>
@@ -5224,10 +5223,10 @@
       <c r="F37">
         <v>9229</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="7">
         <v>1.1100000000000001E-3</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="7" t="s">
         <v>54</v>
       </c>
     </row>
@@ -5247,10 +5246,10 @@
       <c r="F38">
         <v>8578</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="7" t="s">
         <v>44</v>
       </c>
     </row>
@@ -5356,7 +5355,7 @@
   <dimension ref="A1:R44"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C43" activeCellId="1" sqref="C41:E41 C43:E44"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6238,7 +6237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50ACBF76-44B5-4680-9A32-27A43CC564F5}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -6408,7 +6407,6 @@
       <c r="G6">
         <v>0.56399999999999995</v>
       </c>
-      <c r="H6" s="23"/>
       <c r="I6" t="s">
         <v>17</v>
       </c>
@@ -6427,7 +6425,6 @@
       <c r="N6">
         <v>0.81699999999999995</v>
       </c>
-      <c r="O6" s="23"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
@@ -6546,16 +6543,16 @@
       <c r="E12" s="7">
         <v>0.33</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="I12" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="23">
+      <c r="J12">
         <v>0.13</v>
       </c>
-      <c r="K12" s="23">
-        <v>0</v>
-      </c>
-      <c r="L12" s="23">
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
         <v>0.31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
results, figures and table updated
</commit_message>
<xml_diff>
--- a/doc/model results.xlsx
+++ b/doc/model results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/movealong/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="506" documentId="13_ncr:1_{98ABCBFD-7B43-43F9-A7A1-55688472F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DC24151-4B3D-48B2-85C7-6C127FC124DD}"/>
+  <xr:revisionPtr revIDLastSave="507" documentId="13_ncr:1_{98ABCBFD-7B43-43F9-A7A1-55688472F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E2C068A-90E0-411D-998F-22CF5E923E45}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{B02C3BB0-3B4F-4AA3-A8CF-A5D428BFD4B8}"/>
+    <workbookView xWindow="-28485" yWindow="345" windowWidth="13110" windowHeight="14805" activeTab="2" xr2:uid="{B02C3BB0-3B4F-4AA3-A8CF-A5D428BFD4B8}"/>
   </bookViews>
   <sheets>
     <sheet name="autumn_germ" sheetId="2" r:id="rId1"/>
@@ -703,7 +703,7 @@
   <dimension ref="A2:R28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD30"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,7 +1247,7 @@
   <dimension ref="A2:R28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD30"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1795,13 +1795,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C77618-B808-42C0-948C-81CC35016D49}">
   <dimension ref="A2:R28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" customWidth="1"/>
     <col min="8" max="8" width="6.7109375" customWidth="1"/>
     <col min="9" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6.42578125" customWidth="1"/>
@@ -3973,7 +3973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F0277B2-62A9-411E-8838-82E73478C0F2}">
   <dimension ref="A2:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>

</xml_diff>